<commit_message>
plan updated to include story outline
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{928627FF-CC91-4EA5-A79A-17167EC2B1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6085D3-5078-467C-9E2B-0BCB3699B6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>plan begun - main themes and reference images, git/admin stuff, scrolling menu implemented</t>
+  </si>
+  <si>
+    <t>combat implementation - basic parts and placeholder sprites/abiklities</t>
+  </si>
+  <si>
+    <t>combat bugfixes and extra features</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,6 +460,28 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
a beginning on dialogue
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6085D3-5078-467C-9E2B-0BCB3699B6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E19551-B067-462C-B72A-1AA55D78D171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>combat bugfixes and extra features</t>
+  </si>
+  <si>
+    <t>Movement and dialogue system</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,6 +485,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>45617</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tweaks for the dialogue system and bugfixes
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E19551-B067-462C-B72A-1AA55D78D171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E715C105-FD5C-42D7-A7CE-C97122804045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="14400" windowHeight="7815" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,6 +492,14 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>45618</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed a key bug in the dialogue system
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E715C105-FD5C-42D7-A7CE-C97122804045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD30C20-4CF7-4446-84C4-5094349AB749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="14400" windowHeight="7815" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7810" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Movement and dialogue system</t>
+  </si>
+  <si>
+    <t>Impoved dialogue system and added decision support</t>
   </si>
 </sst>
 </file>
@@ -500,6 +503,12 @@
       <c r="A6" s="1">
         <v>45618</v>
       </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
some frontend for dialogue, some work on the inventory
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B71203-3944-47D9-9990-9483590AA6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAB635D-C248-46F8-B78A-3381C6FBAD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19400" windowHeight="11000" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Finished dialogue system functionality &amp; worked on some frontend stuff</t>
+  </si>
+  <si>
+    <t>Some more front end for dialogue and a beginning on the inventory.</t>
   </si>
 </sst>
 </file>
@@ -435,19 +438,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="84.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="84.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45614</v>
       </c>
@@ -469,7 +472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45615</v>
       </c>
@@ -480,7 +483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45616</v>
       </c>
@@ -491,7 +494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45617</v>
       </c>
@@ -502,7 +505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45618</v>
       </c>
@@ -513,7 +516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45621</v>
       </c>
@@ -522,6 +525,17 @@
       </c>
       <c r="C7">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>45622</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redone some backend and implemented some of the inventory backend
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAB635D-C248-46F8-B78A-3381C6FBAD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7A8ACE-1148-4BA6-868A-76A106FAA4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Some more front end for dialogue and a beginning on the inventory.</t>
+  </si>
+  <si>
+    <t>Redoing backend for ui controllers so its easier to use.</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,6 +541,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>45623</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
stone tilemap & items in the inventory & general inventory bugfixes
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7A8ACE-1148-4BA6-868A-76A106FAA4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3A9799-FE70-408C-85DA-10C08F7167A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -68,7 +68,7 @@
     <t>Some more front end for dialogue and a beginning on the inventory.</t>
   </si>
   <si>
-    <t>Redoing backend for ui controllers so its easier to use.</t>
+    <t>Redoing backend for ui controllers so its easier to use. And some frontend for the movement system.</t>
   </si>
 </sst>
 </file>
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,6 +548,14 @@
       <c r="B9" t="s">
         <v>10</v>
       </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>45624</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
improvements on the visuals of the inventory and a beginning oon some of the puzzle mechanics, as well as implementing all the sprites i made so far
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3A9799-FE70-408C-85DA-10C08F7167A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F3041B-5E9E-40C2-8B8F-DDCCCBC84AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11715" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Redoing backend for ui controllers so its easier to use. And some frontend for the movement system.</t>
+  </si>
+  <si>
+    <t>item inventory done, and more front end for both dialogue and te rest of the inventory</t>
   </si>
 </sst>
 </file>
@@ -441,19 +444,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="2" width="84.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45614</v>
       </c>
@@ -475,7 +478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45615</v>
       </c>
@@ -486,7 +489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45616</v>
       </c>
@@ -497,7 +500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45617</v>
       </c>
@@ -508,7 +511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45618</v>
       </c>
@@ -519,7 +522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45621</v>
       </c>
@@ -530,7 +533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45622</v>
       </c>
@@ -541,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45623</v>
       </c>
@@ -552,9 +555,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45624</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redone combat, added it into the main game so far and done some of the spritework for inventory and walking
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F3041B-5E9E-40C2-8B8F-DDCCCBC84AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B738677-737A-4565-9A6F-FB0A455D50FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11715" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7810" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>item inventory done, and more front end for both dialogue and te rest of the inventory</t>
+  </si>
+  <si>
+    <t>improvments on the inventory and a beginning on some puzzle mechanics</t>
   </si>
 </sst>
 </file>
@@ -444,19 +447,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="84.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="84.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45614</v>
       </c>
@@ -478,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45615</v>
       </c>
@@ -489,7 +492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45616</v>
       </c>
@@ -500,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45617</v>
       </c>
@@ -511,7 +514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45618</v>
       </c>
@@ -522,7 +525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45621</v>
       </c>
@@ -533,7 +536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45622</v>
       </c>
@@ -544,7 +547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45623</v>
       </c>
@@ -555,7 +558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45624</v>
       </c>
@@ -566,9 +569,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45625</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>45628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
most changes related to implemetning features for the hot/cold puzzle
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B738677-737A-4565-9A6F-FB0A455D50FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A69649-CDEF-48EB-84EC-8604A0B9421F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7810" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>improvments on the inventory and a beginning on some puzzle mechanics</t>
+  </si>
+  <si>
+    <t>fixing some bugs in the combat system and implementing it into the main area, some more visual for the inventory and the walking animations</t>
+  </si>
+  <si>
+    <t>implemented money and most of the systems required so far for the hot/cold puzzle types</t>
   </si>
 </sst>
 </file>
@@ -447,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -584,6 +590,20 @@
       <c r="A12" s="1">
         <v>45628</v>
       </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>45629</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
a bunch of sprites for the hot/cold puzzle and a start on the overworld combat and the boss ai
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A69649-CDEF-48EB-84EC-8604A0B9421F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F36BCBE-ACA4-4F5D-9A40-5A146FF9E84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7810" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>implemented money and most of the systems required so far for the hot/cold puzzle types</t>
+  </si>
+  <si>
+    <t>done a bunch of spritework for the hot/cold puzzle and began on the first boss pattern and the overworld combat syste,</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -604,6 +607,20 @@
       <c r="B13" t="s">
         <v>14</v>
       </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>45630</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actually started implementing the game - ice puzzle
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447F44E9-AA6F-40F9-92E2-839CD4D5CFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D235CC45-76F7-4CBD-B435-45EF359E1300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7810" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>edges for water tiles sprites done and a boss arena to use, probs for the heat/cold area</t>
+  </si>
+  <si>
+    <t>started an actual boss fight and changes some ideas in the plan</t>
+  </si>
+  <si>
+    <t>finished most of that boss fight and did some spritework on the arena</t>
+  </si>
+  <si>
+    <t>animations for the bossfight</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -650,6 +659,39 @@
         <v>6</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>45635</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>45636</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>45637</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more puzzle stuff and some testing things i wont use (probably)
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D235CC45-76F7-4CBD-B435-45EF359E1300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52374CCC-9ABD-46D1-A681-C1981C9B8128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>animations for the bossfight</t>
+  </si>
+  <si>
+    <t>some animation for the background</t>
+  </si>
+  <si>
+    <t>reworked the player aminator and added holding items as well as a background for the ice puzzle</t>
+  </si>
+  <si>
+    <t>Worked o the aesthetics for the first ice puzzle</t>
   </si>
 </sst>
 </file>
@@ -471,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,6 +701,39 @@
         <v>6</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>45638</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>45639</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>45642</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some more puzzle design and area design
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52374CCC-9ABD-46D1-A681-C1981C9B8128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2010ED45-01E7-4725-968A-661342F7CB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Worked o the aesthetics for the first ice puzzle</t>
+  </si>
+  <si>
+    <t>puzzle design and lore work</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,6 +737,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>45643</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some more making of the first area, + design
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2010ED45-01E7-4725-968A-661342F7CB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6670E37D-F7EA-4712-BFA9-51ED97F788B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>puzzle design and lore work</t>
+  </si>
+  <si>
+    <t>Some work on sprites for the current area and some more puzzles for it too.</t>
   </si>
 </sst>
 </file>
@@ -483,19 +486,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="2" width="84.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45614</v>
       </c>
@@ -517,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45615</v>
       </c>
@@ -528,7 +531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45616</v>
       </c>
@@ -539,7 +542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45617</v>
       </c>
@@ -550,7 +553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45618</v>
       </c>
@@ -561,7 +564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45621</v>
       </c>
@@ -572,7 +575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45622</v>
       </c>
@@ -583,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45623</v>
       </c>
@@ -594,7 +597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45624</v>
       </c>
@@ -605,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45625</v>
       </c>
@@ -616,7 +619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45628</v>
       </c>
@@ -627,7 +630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45629</v>
       </c>
@@ -638,7 +641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45630</v>
       </c>
@@ -649,7 +652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45631</v>
       </c>
@@ -660,7 +663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45632</v>
       </c>
@@ -671,7 +674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45635</v>
       </c>
@@ -682,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45636</v>
       </c>
@@ -693,7 +696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45637</v>
       </c>
@@ -704,7 +707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45638</v>
       </c>
@@ -715,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45639</v>
       </c>
@@ -726,7 +729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45642</v>
       </c>
@@ -737,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45643</v>
       </c>
@@ -746,6 +749,17 @@
       </c>
       <c r="C23">
         <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45644</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
crowlder (some more fleshing out of the current area)
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6670E37D-F7EA-4712-BFA9-51ED97F788B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B04BB-F6C1-476A-BC89-403247CA78A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Some work on sprites for the current area and some more puzzles for it too.</t>
+  </si>
+  <si>
+    <t>Working on the first area in the game</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,6 +765,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45653</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished the crowlder part and added more aniumations to the environment
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B04BB-F6C1-476A-BC89-403247CA78A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489EDD07-EB18-41DC-86A3-0836B80C3634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Working on the first area in the game</t>
+  </si>
+  <si>
+    <t>Fleshing out area more with intereactable objects etc.</t>
   </si>
 </sst>
 </file>
@@ -489,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,6 +779,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45656</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
testing, polishing and rat for current area
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489EDD07-EB18-41DC-86A3-0836B80C3634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC984010-9F6C-47B3-B583-B4E15BC78B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Fleshing out area more with intereactable objects etc.</t>
+  </si>
+  <si>
+    <t>animation for the background and finished crow arc</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,6 +793,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>46022</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
starting on the next section of the area
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC984010-9F6C-47B3-B583-B4E15BC78B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB53513F-8A75-43EE-B7AA-7782FE95C0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>animation for the background and finished crow arc</t>
+  </si>
+  <si>
+    <t>testing, polishing and rat</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,6 +807,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45659</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
a bunch of sprites for the 2nd character"
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB53513F-8A75-43EE-B7AA-7782FE95C0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795FB3E9-6408-4CCD-BC93-DEBFBE316495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>testing, polishing and rat</t>
+  </si>
+  <si>
+    <t>Started on the next part of the area, with some spritework</t>
   </si>
 </sst>
 </file>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,6 +821,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45660</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
mostly reworking the story
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795FB3E9-6408-4CCD-BC93-DEBFBE316495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D7207F-CBE3-4292-9F5F-F66FFCD08C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Started on the next part of the area, with some spritework</t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
+    <t>more writing and planning - reworked one of the characters and the beginning of the story</t>
   </si>
 </sst>
 </file>
@@ -501,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,6 +834,31 @@
       <c r="B29" t="s">
         <v>30</v>
       </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45663</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>45664</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on the mansiona rea
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D7207F-CBE3-4292-9F5F-F66FFCD08C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7FF53A-685B-4463-8037-40FB1A9D4378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
more work on the area
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7FF53A-685B-4463-8037-40FB1A9D4378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F64808-74D5-4533-B6BE-24F29A8731D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>more writing and planning - reworked one of the characters and the beginning of the story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding more content to the current area </t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,6 +863,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>45665</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rest of the mansion (almost) complete
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F64808-74D5-4533-B6BE-24F29A8731D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732A339A-507B-4811-BB18-BF8653C9627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t xml:space="preserve">Adding more content to the current area </t>
+  </si>
+  <si>
+    <t>Upstairs mansion and implementing enemy</t>
   </si>
 </sst>
 </file>
@@ -510,19 +513,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="84.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="84.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45614</v>
       </c>
@@ -544,7 +547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45615</v>
       </c>
@@ -555,7 +558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45616</v>
       </c>
@@ -566,7 +569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45617</v>
       </c>
@@ -577,7 +580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45618</v>
       </c>
@@ -588,7 +591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45621</v>
       </c>
@@ -599,7 +602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45622</v>
       </c>
@@ -610,7 +613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45623</v>
       </c>
@@ -621,7 +624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45624</v>
       </c>
@@ -632,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45625</v>
       </c>
@@ -643,7 +646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45628</v>
       </c>
@@ -654,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>45629</v>
       </c>
@@ -665,7 +668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>45630</v>
       </c>
@@ -676,7 +679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45631</v>
       </c>
@@ -687,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45632</v>
       </c>
@@ -698,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>45635</v>
       </c>
@@ -709,7 +712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>45636</v>
       </c>
@@ -720,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>45637</v>
       </c>
@@ -731,7 +734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>45638</v>
       </c>
@@ -742,7 +745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>45639</v>
       </c>
@@ -753,7 +756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>45642</v>
       </c>
@@ -764,7 +767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45643</v>
       </c>
@@ -775,7 +778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45644</v>
       </c>
@@ -786,7 +789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>45653</v>
       </c>
@@ -797,7 +800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>45656</v>
       </c>
@@ -808,7 +811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>46022</v>
       </c>
@@ -819,7 +822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45659</v>
       </c>
@@ -830,7 +833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45660</v>
       </c>
@@ -841,7 +844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45663</v>
       </c>
@@ -852,7 +855,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45664</v>
       </c>
@@ -863,7 +866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45665</v>
       </c>
@@ -872,6 +875,17 @@
       </c>
       <c r="C32">
         <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>45666</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished mansion (for now)
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732A339A-507B-4811-BB18-BF8653C9627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB8FC56-EADD-4B84-BF62-38916A3A8947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Upstairs mansion and implementing enemy</t>
+  </si>
+  <si>
+    <t>mansion basement</t>
   </si>
 </sst>
 </file>
@@ -513,19 +516,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="2" width="84.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45614</v>
       </c>
@@ -547,7 +550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45615</v>
       </c>
@@ -558,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45616</v>
       </c>
@@ -569,7 +572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45617</v>
       </c>
@@ -580,7 +583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45618</v>
       </c>
@@ -591,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45621</v>
       </c>
@@ -602,7 +605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45622</v>
       </c>
@@ -613,7 +616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45623</v>
       </c>
@@ -624,7 +627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45624</v>
       </c>
@@ -635,7 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45625</v>
       </c>
@@ -646,7 +649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45628</v>
       </c>
@@ -657,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45629</v>
       </c>
@@ -668,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45630</v>
       </c>
@@ -679,7 +682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45631</v>
       </c>
@@ -690,7 +693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45632</v>
       </c>
@@ -701,7 +704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45635</v>
       </c>
@@ -712,7 +715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45636</v>
       </c>
@@ -723,7 +726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45637</v>
       </c>
@@ -734,7 +737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45638</v>
       </c>
@@ -745,7 +748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45639</v>
       </c>
@@ -756,7 +759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45642</v>
       </c>
@@ -767,7 +770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45643</v>
       </c>
@@ -778,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45644</v>
       </c>
@@ -789,7 +792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45653</v>
       </c>
@@ -800,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45656</v>
       </c>
@@ -811,7 +814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>46022</v>
       </c>
@@ -822,7 +825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45659</v>
       </c>
@@ -833,7 +836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45660</v>
       </c>
@@ -844,7 +847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45663</v>
       </c>
@@ -855,7 +858,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45664</v>
       </c>
@@ -866,7 +869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45665</v>
       </c>
@@ -877,7 +880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45666</v>
       </c>
@@ -886,6 +889,17 @@
       </c>
       <c r="C33">
         <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
beginning on next area as well as fleshing out older area
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB8FC56-EADD-4B84-BF62-38916A3A8947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A12E46F-C812-4AD0-B1C8-EB164E014EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>mansion basement</t>
+  </si>
+  <si>
+    <t>finshed mansion area</t>
   </si>
 </sst>
 </file>
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,6 +905,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>45670</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some story rewriting and fleshing out areas
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A12E46F-C812-4AD0-B1C8-EB164E014EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ECC9FB-6E43-4114-A46D-29E4CFD74AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>finshed mansion area</t>
+  </si>
+  <si>
+    <t>fleshing out all made areas so far</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,6 +919,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>45671</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some animations for the bossfight and adding more content tot he start
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ECC9FB-6E43-4114-A46D-29E4CFD74AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2237C71-6EE6-4D67-8D0F-7F4F91DF95CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>fleshing out all made areas so far</t>
+  </si>
+  <si>
+    <t>reworking plan for story</t>
   </si>
 </sst>
 </file>
@@ -522,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,6 +933,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>45672</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
library and book donation and some bugfixes
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114BA46E-996C-4D49-8243-1947AA31E612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3809EF4-304C-4D16-A222-DE977ECEDE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11715" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -531,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,7 +974,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>45675</v>
+        <v>45677</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
@@ -982,6 +982,20 @@
       <c r="C40">
         <v>5</v>
       </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>45678</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug fixes and city area
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460B8F51-6D41-42A7-BC87-86526FA583BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112DEBF8-7061-4160-A65A-936238B1AF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11715" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>library book donation</t>
+  </si>
+  <si>
+    <t>butfixes</t>
+  </si>
+  <si>
+    <t>testing out some new ideas</t>
   </si>
 </sst>
 </file>
@@ -534,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,6 +1014,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>45680</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>45681</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
switching render pipleins and stuff for that
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F48010B-C8D4-442F-B477-CBE6A2016260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D08820-41ED-4A9B-921E-EB20D87F03FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>implementing city</t>
+  </si>
+  <si>
+    <t>city art</t>
   </si>
 </sst>
 </file>
@@ -546,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,6 +1067,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45686</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more fleshing out of content
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D08820-41ED-4A9B-921E-EB20D87F03FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D9D563-F6F5-4D81-9CB8-5F0D53FF99EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>city art</t>
+  </si>
+  <si>
+    <t>reconfiguring unity stuff</t>
   </si>
 </sst>
 </file>
@@ -549,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,6 +1081,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>45687</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
library finished (mostly) and the tree stuff
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658ED9E0-5C96-443E-873C-FA04DA6C8D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1424C74-76D2-43E1-842D-FE80657DED6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>visuals stuff</t>
+  </si>
+  <si>
+    <t>library storyline</t>
   </si>
 </sst>
 </file>
@@ -561,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,6 +1137,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>45693</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
starting on the next boss
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\_summergame\pilus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0633F203-73D7-4FE2-B4B4-D214F21124D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFA231B-C4A8-4916-80D7-88390EEB87A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50A7EF49-A95C-4DE8-89ED-112A97A45408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>townhall area</t>
+  </si>
+  <si>
+    <t>continuing with the area</t>
   </si>
 </sst>
 </file>
@@ -573,19 +576,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531B29E5-0107-47AB-96DE-7537903C25B2}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="2" width="84.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45614</v>
       </c>
@@ -607,7 +610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45615</v>
       </c>
@@ -618,7 +621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45616</v>
       </c>
@@ -629,7 +632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45617</v>
       </c>
@@ -640,7 +643,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45618</v>
       </c>
@@ -651,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45621</v>
       </c>
@@ -662,7 +665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45622</v>
       </c>
@@ -673,7 +676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45623</v>
       </c>
@@ -684,7 +687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45624</v>
       </c>
@@ -695,7 +698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45625</v>
       </c>
@@ -706,7 +709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45628</v>
       </c>
@@ -717,7 +720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45629</v>
       </c>
@@ -728,7 +731,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45630</v>
       </c>
@@ -739,7 +742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45631</v>
       </c>
@@ -750,7 +753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45632</v>
       </c>
@@ -761,7 +764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45635</v>
       </c>
@@ -772,7 +775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45636</v>
       </c>
@@ -783,7 +786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45637</v>
       </c>
@@ -794,7 +797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45638</v>
       </c>
@@ -805,7 +808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45639</v>
       </c>
@@ -816,7 +819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45642</v>
       </c>
@@ -827,7 +830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45643</v>
       </c>
@@ -838,7 +841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45644</v>
       </c>
@@ -849,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45653</v>
       </c>
@@ -860,7 +863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45656</v>
       </c>
@@ -871,7 +874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>46022</v>
       </c>
@@ -882,7 +885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45659</v>
       </c>
@@ -893,7 +896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45660</v>
       </c>
@@ -904,7 +907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45663</v>
       </c>
@@ -915,7 +918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45664</v>
       </c>
@@ -926,7 +929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45665</v>
       </c>
@@ -937,7 +940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45666</v>
       </c>
@@ -948,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45667</v>
       </c>
@@ -959,7 +962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45670</v>
       </c>
@@ -970,7 +973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45671</v>
       </c>
@@ -981,7 +984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45672</v>
       </c>
@@ -992,7 +995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45673</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45674</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45677</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45678</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45679</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45680</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45681</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45684</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45685</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45686</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45687</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45688</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45691</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45692</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45693</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45695</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45698</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45700</v>
       </c>
@@ -1187,6 +1190,17 @@
         <v>54</v>
       </c>
       <c r="C55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>45702</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56">
         <v>4</v>
       </c>
     </row>

</xml_diff>